<commit_message>
store carport dim in fog.Order
</commit_message>
<xml_diff>
--- a/partlist for db.xlsx
+++ b/partlist for db.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" calcCompleted="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="55">
   <si>
     <t>fædigskåret</t>
   </si>
@@ -139,6 +139,51 @@
   </si>
   <si>
     <t>standardPrice</t>
+  </si>
+  <si>
+    <t>45x195 mm. ubh. Spaertrae</t>
+  </si>
+  <si>
+    <t>19x100 mm. trykimp. Braet</t>
+  </si>
+  <si>
+    <t>1x20 mm. hulband 10 mtr.</t>
+  </si>
+  <si>
+    <t>universal hojre</t>
+  </si>
+  <si>
+    <t>10x120 mm. Braeddebolt</t>
+  </si>
+  <si>
+    <t>50x75 mm. Stalddorsgreb</t>
+  </si>
+  <si>
+    <t>t-haengsel</t>
+  </si>
+  <si>
+    <t>25x150 mm. trykimp. Braet</t>
+  </si>
+  <si>
+    <t>faedigskaret</t>
+  </si>
+  <si>
+    <t>25x50 mm. trykimp. Braet</t>
+  </si>
+  <si>
+    <t>B&amp;C Toplaegte holder</t>
+  </si>
+  <si>
+    <t>25x125 mm. trykimp. Braet</t>
+  </si>
+  <si>
+    <t>25x200 mm. trykimp. Braet</t>
+  </si>
+  <si>
+    <t>38x73 mm. Laegte</t>
+  </si>
+  <si>
+    <t>38x73 mm. Taglaegte T1</t>
   </si>
 </sst>
 </file>
@@ -527,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -538,7 +583,7 @@
     <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -549,7 +594,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -559,8 +604,11 @@
       <c r="C2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -570,8 +618,11 @@
       <c r="C3">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -582,7 +633,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -592,8 +643,11 @@
       <c r="C5">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -604,7 +658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -614,8 +668,11 @@
       <c r="C7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -625,8 +682,11 @@
       <c r="C8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -636,8 +696,11 @@
       <c r="C9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -647,8 +710,11 @@
       <c r="C10">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -658,8 +724,11 @@
       <c r="C11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -670,7 +739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -680,8 +749,11 @@
       <c r="C13">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -692,7 +764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -703,7 +775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -713,8 +785,11 @@
       <c r="C17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -725,7 +800,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -736,7 +811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -746,8 +821,11 @@
       <c r="C20">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -758,7 +836,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -768,8 +846,11 @@
       <c r="C22">
         <v>200</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -779,8 +860,11 @@
       <c r="C23">
         <v>300</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -791,7 +875,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -802,7 +886,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -813,7 +897,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -824,7 +908,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -834,8 +918,11 @@
       <c r="C28">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -846,7 +933,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -857,7 +944,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -868,7 +955,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -879,7 +966,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -889,8 +976,11 @@
       <c r="C33">
         <v>100</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -901,7 +991,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -912,7 +1002,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
first try random salesRep id
</commit_message>
<xml_diff>
--- a/partlist for db.xlsx
+++ b/partlist for db.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28060" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="18880" yWindow="0" windowWidth="9100" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" calcCompleted="0" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,29 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="55">
-  <si>
-    <t>fædigskåret</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
   <si>
     <t>97x97 mm. trykimp. Stolpe</t>
   </si>
   <si>
-    <t>25x150 mm. trykimp. Bræt</t>
-  </si>
-  <si>
-    <t>45x195 mm. ubh. Spærtræ</t>
-  </si>
-  <si>
-    <t>19x100 mm. trykimp. Bræt</t>
-  </si>
-  <si>
-    <t>25x50 mm. trykimp. Bræt</t>
-  </si>
-  <si>
-    <t>38x73 mm. taglægte T1</t>
-  </si>
-  <si>
     <t>WOOD</t>
   </si>
   <si>
@@ -54,30 +36,18 @@
     <t>B&amp;C Rygsten sort</t>
   </si>
   <si>
-    <t>B&amp;C Toplægte holder</t>
-  </si>
-  <si>
     <t>B&amp;C Rygstensbeslag</t>
   </si>
   <si>
     <t>B&amp;C Tagstensbindere &amp; nakkekroge</t>
   </si>
   <si>
-    <t>universal højre</t>
-  </si>
-  <si>
     <t>SCREW</t>
   </si>
   <si>
     <t>universal venstre</t>
   </si>
   <si>
-    <t>50x75 mm. Stalddørsgreb</t>
-  </si>
-  <si>
-    <t>t-hængsel</t>
-  </si>
-  <si>
     <t>vinkelbeslag</t>
   </si>
   <si>
@@ -90,9 +60,6 @@
     <t>5x100 mm. skruer 100 stk.</t>
   </si>
   <si>
-    <t>10x120 mm. Bræddebolt</t>
-  </si>
-  <si>
     <t>40x40 mm. firkantskiver</t>
   </si>
   <si>
@@ -105,21 +72,12 @@
     <t>45x95 mm. ubh. Reglar</t>
   </si>
   <si>
-    <t>25x200 mm. trykimp. Bræt</t>
-  </si>
-  <si>
-    <t>25x125 mm. trykimp. Bræt</t>
-  </si>
-  <si>
     <t>Plastmo Ecolite Blue</t>
   </si>
   <si>
     <t>Plastmo bundskruer 200 stk.</t>
   </si>
   <si>
-    <t>1x20 mm. hulbånd 10 mtr.</t>
-  </si>
-  <si>
     <t>4x50 mm. beslagskruer 250 stk.</t>
   </si>
   <si>
@@ -127,9 +85,6 @@
   </si>
   <si>
     <t>4,5x50 mm. skruer 300 stk.</t>
-  </si>
-  <si>
-    <t>38x73 mm. Lægte</t>
   </si>
   <si>
     <t>type</t>
@@ -215,12 +170,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -237,8 +198,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Besøgt link" xfId="2" builtinId="9" hidden="1"/>
@@ -572,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -583,431 +545,386 @@
     <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C3">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C4">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C5">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C7">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="C9">
         <v>6</v>
       </c>
-      <c r="D9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C10">
         <v>12</v>
       </c>
-      <c r="D10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C11">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C13">
         <v>6</v>
       </c>
-      <c r="D13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C16">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
-      <c r="D17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C18">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C19">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C20">
         <v>10</v>
       </c>
-      <c r="D20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C21">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C22">
         <v>200</v>
       </c>
-      <c r="D22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C23">
         <v>300</v>
       </c>
-      <c r="D23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C24">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" t="s">
-        <v>20</v>
+        <v>7</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C25">
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" t="s">
-        <v>21</v>
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C26">
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" t="s">
-        <v>22</v>
+        <v>7</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C27">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C28">
         <v>20</v>
       </c>
-      <c r="D28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" t="s">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C29">
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" t="s">
-        <v>25</v>
+        <v>7</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C30">
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B31" t="s">
-        <v>26</v>
       </c>
       <c r="C31">
         <v>350</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" t="s">
-        <v>31</v>
+        <v>7</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C32">
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" t="s">
-        <v>32</v>
+        <v>7</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C33">
         <v>100</v>
       </c>
-      <c r="D33" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" t="s">
-        <v>33</v>
+        <v>7</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C34">
         <v>250</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" t="s">
-        <v>34</v>
+        <v>7</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C35">
         <v>400</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>15</v>
-      </c>
-      <c r="B36" t="s">
-        <v>35</v>
+        <v>7</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C36">
         <v>300</v>

</xml_diff>